<commit_message>
new room tables created
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
     <sheet name="UnlockableThief" sheetId="2" r:id="rId2"/>
     <sheet name="UnlockableItem" sheetId="1" r:id="rId3"/>
     <sheet name="ThiefLevel" sheetId="4" r:id="rId4"/>
-    <sheet name="CastleRooms" sheetId="9" r:id="rId5"/>
-    <sheet name="RoomUpgrades" sheetId="11" r:id="rId6"/>
-    <sheet name="ThroneUpgrades" sheetId="3" r:id="rId7"/>
-    <sheet name="BasicRooms" sheetId="10" r:id="rId8"/>
-    <sheet name="AdvancedRooms" sheetId="8" r:id="rId9"/>
+    <sheet name="CastleRoom" sheetId="9" r:id="rId5"/>
+    <sheet name="RoomUpgrade" sheetId="11" r:id="rId6"/>
+    <sheet name="ThroneRoom" sheetId="3" r:id="rId7"/>
+    <sheet name="BasicRoom" sheetId="10" r:id="rId8"/>
+    <sheet name="AdvancedRoom" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="192">
   <si>
     <t>Class</t>
   </si>
@@ -281,111 +281,6 @@
     <t>30 sec</t>
   </si>
   <si>
-    <t>BonusGold</t>
-  </si>
-  <si>
-    <t>DailySlots</t>
-  </si>
-  <si>
-    <t>BonusGems</t>
-  </si>
-  <si>
-    <t>UnlockSlots</t>
-  </si>
-  <si>
-    <t>BonusMaterials</t>
-  </si>
-  <si>
-    <t>BonusXP</t>
-  </si>
-  <si>
-    <t>FenceStaff</t>
-  </si>
-  <si>
-    <t>JewelerStaff</t>
-  </si>
-  <si>
-    <t>WorkshopStaff</t>
-  </si>
-  <si>
-    <t>ReformatoryStaff</t>
-  </si>
-  <si>
-    <t>+1% per 3 END</t>
-  </si>
-  <si>
-    <t>+2% per 3 END</t>
-  </si>
-  <si>
-    <t>+3% per 3 END</t>
-  </si>
-  <si>
-    <t>+4% per 3 END</t>
-  </si>
-  <si>
-    <t>+5% per 3 END</t>
-  </si>
-  <si>
-    <t>+6% per 3 END</t>
-  </si>
-  <si>
-    <t>+7% per 3 END</t>
-  </si>
-  <si>
-    <t>+4% per 5 MIG</t>
-  </si>
-  <si>
-    <t>+6% per 5 MIG</t>
-  </si>
-  <si>
-    <t>+8% per 5 MIG</t>
-  </si>
-  <si>
-    <t>+10% per 5 MIG</t>
-  </si>
-  <si>
-    <t>+12% per 5 MIG</t>
-  </si>
-  <si>
-    <t>+14% per 5 MIG</t>
-  </si>
-  <si>
-    <t>+16% per 5 MIG</t>
-  </si>
-  <si>
-    <t>+1% per 5 AGI</t>
-  </si>
-  <si>
-    <t>+3% per 5 AGI</t>
-  </si>
-  <si>
-    <t>+4% per 5 AGI</t>
-  </si>
-  <si>
-    <t>+5% per 5 AGI</t>
-  </si>
-  <si>
-    <t>+6% per 5 AGI</t>
-  </si>
-  <si>
-    <t>+2% per 5 AGI</t>
-  </si>
-  <si>
-    <t>+30% per 5 CUN</t>
-  </si>
-  <si>
-    <t>+15% per 5 CUN</t>
-  </si>
-  <si>
-    <t>+45% per 5 CUN</t>
-  </si>
-  <si>
-    <t>+60% per 5 CUN</t>
-  </si>
-  <si>
-    <t>+75% per 5 CUN</t>
-  </si>
-  <si>
     <t>StartTrait</t>
   </si>
   <si>
@@ -498,12 +393,6 @@
   </si>
   <si>
     <t>Dorm_Recovery</t>
-  </si>
-  <si>
-    <t>Exped_Slots</t>
-  </si>
-  <si>
-    <t>Exped_SpeedUp</t>
   </si>
   <si>
     <t>AllowedPlacement</t>
@@ -667,6 +556,54 @@
   </si>
   <si>
     <t>end 3</t>
+  </si>
+  <si>
+    <t>Cartog_Slots</t>
+  </si>
+  <si>
+    <t>Cartog_Recovery</t>
+  </si>
+  <si>
+    <t>Fence_GoldBonus</t>
+  </si>
+  <si>
+    <t>Fence_MagicSlots</t>
+  </si>
+  <si>
+    <t>Workshop_StoneBonus</t>
+  </si>
+  <si>
+    <t>Workshop_Defense</t>
+  </si>
+  <si>
+    <t>trap +1</t>
+  </si>
+  <si>
+    <t>thief +1</t>
+  </si>
+  <si>
+    <t>Jeweler_GemBonus</t>
+  </si>
+  <si>
+    <t>Jeweler_ExpedSlots</t>
+  </si>
+  <si>
+    <t>Artisan_Cost</t>
+  </si>
+  <si>
+    <t>Artisan_Period</t>
+  </si>
+  <si>
+    <t>Blacksmith_Period</t>
+  </si>
+  <si>
+    <t>20 hr</t>
+  </si>
+  <si>
+    <t>trap +2</t>
+  </si>
+  <si>
+    <t>thief +2</t>
   </si>
 </sst>
 </file>
@@ -1088,17 +1025,17 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1275,13 +1212,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -1365,7 +1302,7 @@
         <v>6700</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -1386,7 +1323,7 @@
         <v>6700</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -1407,7 +1344,7 @@
         <v>6700</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -1428,7 +1365,7 @@
         <v>11400</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
@@ -1449,7 +1386,7 @@
         <v>11400</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
@@ -1470,7 +1407,7 @@
         <v>11400</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="F10" s="1">
         <v>4</v>
@@ -1491,7 +1428,7 @@
         <v>17100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="F11" s="1">
         <v>6</v>
@@ -1512,7 +1449,7 @@
         <v>17100</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="F12" s="1">
         <v>6</v>
@@ -1533,7 +1470,7 @@
         <v>17100</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="F13" s="1">
         <v>6</v>
@@ -1549,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
@@ -1570,16 +1507,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>24</v>
@@ -1600,7 +1537,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1851,7 +1788,7 @@
         <v>600</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1879,7 +1816,7 @@
         <v>600</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1907,7 +1844,7 @@
         <v>600</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1940,7 +1877,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1996,7 +1933,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -2012,14 +1949,14 @@
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="G15" s="5">
         <f>VLOOKUP(E15, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2056,7 +1993,7 @@
         <v>42</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2093,7 +2030,7 @@
         <v>44</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2131,7 +2068,7 @@
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="8" t="s">
-        <v>204</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2168,7 +2105,7 @@
         <v>43</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2205,7 +2142,7 @@
         <v>45</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2242,7 +2179,7 @@
         <v>46</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2270,10 +2207,10 @@
         <v>1300</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2301,10 +2238,10 @@
         <v>1300</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2332,10 +2269,10 @@
         <v>1300</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2366,12 +2303,12 @@
         <v>46</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -2397,7 +2334,7 @@
         <v>42</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2428,12 +2365,12 @@
         <v>48</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2449,17 +2386,17 @@
         <v>2</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="G29" s="5">
         <f>VLOOKUP(E29, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2692,7 +2629,7 @@
         <v>1300</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2720,7 +2657,7 @@
         <v>1300</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2748,7 +2685,7 @@
         <v>1300</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -2781,7 +2718,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B41" s="1">
         <v>2</v>
@@ -2837,7 +2774,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="B43" s="1">
         <v>2</v>
@@ -2853,14 +2790,14 @@
         <v>2</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="G43" s="5">
         <f>VLOOKUP(E43, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2897,7 +2834,7 @@
         <v>42</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2934,7 +2871,7 @@
         <v>44</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -2972,7 +2909,7 @@
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="8" t="s">
-        <v>204</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -3009,7 +2946,7 @@
         <v>43</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -3046,7 +2983,7 @@
         <v>45</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -3083,7 +3020,7 @@
         <v>46</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -3111,10 +3048,10 @@
         <v>2100</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -3142,10 +3079,10 @@
         <v>2100</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -3173,10 +3110,10 @@
         <v>2100</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -3207,12 +3144,12 @@
         <v>45</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B55" s="1">
         <v>2</v>
@@ -3238,7 +3175,7 @@
         <v>52</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -3269,12 +3206,12 @@
         <v>44</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="B57" s="1">
         <v>2</v>
@@ -3290,17 +3227,17 @@
         <v>3</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="G57" s="5">
         <f>VLOOKUP(E57, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3622,7 +3559,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B69" s="1">
         <v>3</v>
@@ -3678,7 +3615,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="B71" s="1">
         <v>3</v>
@@ -3694,14 +3631,14 @@
         <v>3</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="G71" s="5">
         <f>VLOOKUP(E71, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -3738,7 +3675,7 @@
         <v>42</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -3775,7 +3712,7 @@
         <v>44</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -3813,7 +3750,7 @@
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="8" t="s">
-        <v>204</v>
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -3850,7 +3787,7 @@
         <v>43</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -3887,7 +3824,7 @@
         <v>45</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -3924,7 +3861,7 @@
         <v>46</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -3955,7 +3892,7 @@
         <v>53</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -3986,7 +3923,7 @@
         <v>54</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -4017,7 +3954,7 @@
         <v>55</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -4048,12 +3985,12 @@
         <v>43</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B83" s="1">
         <v>3</v>
@@ -4079,7 +4016,7 @@
         <v>59</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
@@ -4110,12 +4047,12 @@
         <v>47</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="B85" s="1">
         <v>1</v>
@@ -4130,16 +4067,16 @@
         <v>2</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="G85" s="1">
         <v>1300</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -4210,7 +4147,7 @@
         <v>83</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4235,7 +4172,7 @@
         <v>61</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -4254,10 +4191,10 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>63</v>
@@ -4282,7 +4219,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>64</v>
@@ -4479,7 +4416,7 @@
         <v>290</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>15</v>
@@ -4524,180 +4461,180 @@
         <v>3</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="B2" s="19">
         <v>1</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="B3" s="19">
         <v>1</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="B4" s="19">
         <v>3</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="B6" s="19">
         <v>1</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="B7" s="19">
         <v>1</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="B8" s="19">
         <v>1</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="B9" s="19">
         <v>2</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="B10" s="19">
         <v>2</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>168</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>179</v>
+        <v>142</v>
       </c>
       <c r="B12" s="19">
         <v>4</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="B13" s="19">
         <v>4</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B14" s="19">
         <v>4</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>185</v>
+        <v>148</v>
       </c>
       <c r="B15" s="19">
         <v>4</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>186</v>
+        <v>149</v>
       </c>
       <c r="B16" s="19">
         <v>4</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4726,22 +4663,22 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4764,7 +4701,7 @@
         <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4785,10 +4722,10 @@
         <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -4884,7 +4821,7 @@
         <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -4905,7 +4842,7 @@
         <v>76</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>77</v>
@@ -4926,13 +4863,13 @@
         <v>5900</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -4953,7 +4890,7 @@
         <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>78</v>
@@ -4967,7 +4904,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -4994,15 +4931,18 @@
         <v>81</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>197</v>
+        <v>160</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>198</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:C10" si="0">A2</f>
@@ -5023,6 +4963,10 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
+      <c r="B3" s="1">
+        <f>B2+1</f>
+        <v>7</v>
+      </c>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -5044,12 +4988,16 @@
         <f t="shared" ref="A4:A10" si="2">A3+1</f>
         <v>3</v>
       </c>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B10" si="3">B3+1</f>
+        <v>8</v>
+      </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ref="D4:D10" si="3">D3+0.5</f>
+        <f t="shared" ref="D4:D10" si="4">D3+0.5</f>
         <v>7</v>
       </c>
       <c r="E4" s="10">
@@ -5065,12 +5013,15 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="B5" s="1">
+        <v>8</v>
+      </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D5" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.5</v>
       </c>
       <c r="E5" s="10">
@@ -5086,12 +5037,16 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="B6" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D6" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="E6" s="10">
@@ -5107,12 +5062,16 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="B7" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D7" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5</v>
       </c>
       <c r="E7" s="10">
@@ -5128,12 +5087,15 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
+      <c r="B8" s="1">
+        <v>10</v>
+      </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D8" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="E8" s="10">
@@ -5149,12 +5111,16 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="B9" s="1">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D9" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.5</v>
       </c>
       <c r="E9" s="10">
@@ -5170,12 +5136,16 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
+      <c r="B10" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="D10" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="E10" s="10">
@@ -5184,57 +5154,6 @@
       </c>
       <c r="F10" s="10">
         <v>2600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="1">
-        <f>B11+1</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <f t="shared" ref="B13:B19" si="4">B12+1</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="1">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
-        <f t="shared" si="4"/>
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5258,7 +5177,8 @@
     <col min="5" max="5" width="16.77734375" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="14.77734375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="14.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5267,31 +5187,31 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -5317,13 +5237,15 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
+      <c r="H2" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="I2" s="11">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -5355,6 +5277,9 @@
       <c r="I3" s="1">
         <v>1</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -5386,6 +5311,9 @@
       <c r="I4" s="1">
         <v>1</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -5412,10 +5340,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -5443,10 +5374,13 @@
         <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="I6" s="1">
         <v>2</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -5479,6 +5413,9 @@
       <c r="I7" s="1">
         <v>2</v>
       </c>
+      <c r="J7" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -5510,6 +5447,9 @@
       <c r="I8" s="1">
         <v>2</v>
       </c>
+      <c r="J8" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -5536,10 +5476,13 @@
         <v>4</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="I9" s="1">
         <v>3</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -5567,10 +5510,13 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="I10" s="1">
         <v>3</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -5602,181 +5548,174 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" style="1" customWidth="1"/>
-    <col min="2" max="4" width="14.77734375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="14.77734375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="14" customWidth="1"/>
-    <col min="8" max="10" width="14.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.77734375" customWidth="1"/>
+    <col min="2" max="3" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="14" customWidth="1"/>
+    <col min="6" max="7" width="17.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>85</v>
+        <v>179</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>91</v>
+        <v>185</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>108</v>
+      <c r="B2" s="1">
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="F2" s="14">
         <v>1</v>
       </c>
       <c r="G2" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="I2" s="10">
+        <f xml:space="preserve"> cost!C4 - cost!C3</f>
+        <v>700</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>113</v>
+      <c r="B3" s="1">
+        <f>B2 +2</f>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <f>D2 +2</f>
+        <v>6</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>114</v>
+        <v>182</v>
       </c>
       <c r="F3" s="14">
         <v>1</v>
       </c>
       <c r="G3" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="I3" s="10">
+        <f xml:space="preserve"> cost!C5 - cost!C4</f>
+        <v>800</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>109</v>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:D10" si="1">B3 +2</f>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>114</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E4" s="13"/>
       <c r="F4" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="14">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="10">
+        <f xml:space="preserve"> cost!C6 - cost!C5</f>
+        <v>1000</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>109</v>
+      <c r="B5" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="F5" s="14">
         <v>2</v>
@@ -5784,198 +5723,199 @@
       <c r="G5" s="14">
         <v>1</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="1">
-        <v>2</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="10">
+        <f xml:space="preserve"> cost!C7 - cost!C6</f>
+        <v>1100</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>110</v>
+      <c r="B6" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>116</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E6" s="13"/>
       <c r="F6" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" s="14">
         <v>1</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" s="1">
-        <v>2</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="K6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I6" s="10">
+        <f xml:space="preserve"> cost!C8 - cost!C7</f>
+        <v>1200</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>110</v>
+      <c r="B7" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>116</v>
+        <v>190</v>
       </c>
       <c r="F7" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="14">
-        <v>2</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="K7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="10">
+        <f xml:space="preserve"> cost!C9 - cost!C8</f>
+        <v>1300</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>110</v>
+      <c r="B8" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>117</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E8" s="13"/>
       <c r="F8" s="14">
         <v>3</v>
       </c>
       <c r="G8" s="14">
         <v>2</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="I8" s="1">
-        <v>3</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="K8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="10">
+        <f xml:space="preserve"> cost!C10 - cost!C9</f>
+        <v>1400</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>111</v>
+      <c r="B9" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>117</v>
+        <v>191</v>
       </c>
       <c r="F9" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="14">
         <v>2</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="I9" s="1">
-        <v>3</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="K9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="10">
+        <f xml:space="preserve"> cost!C11 - cost!C10</f>
+        <v>1600</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>112</v>
+      <c r="B10" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
-        <v>2</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>118</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E10" s="13"/>
       <c r="F10" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="14">
         <v>2</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" s="1">
-        <v>3</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="K10" s="1">
-        <v>3</v>
-      </c>
+      <c r="H10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I10" s="10">
+        <f xml:space="preserve"> cost!C12 - cost!C11</f>
+        <v>1700</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E13" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
materials reduced to just stone
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4130,8 +4130,8 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="10">
-        <v>200</v>
+      <c r="B2" s="1">
+        <v>0</v>
       </c>
       <c r="C2" s="10">
         <v>12</v>
@@ -4156,7 +4156,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="C3" s="10">
         <v>26</v>
@@ -4181,7 +4181,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10">
-        <v>1200</v>
+        <v>600</v>
       </c>
       <c r="C4" s="10">
         <v>42</v>
@@ -4206,7 +4206,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10">
-        <v>2000</v>
+        <v>1200</v>
       </c>
       <c r="C5" s="10">
         <v>62</v>
@@ -4231,7 +4231,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C6" s="10">
         <v>84</v>
@@ -4256,7 +4256,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10">
-        <v>4200</v>
+        <v>3000</v>
       </c>
       <c r="C7" s="10">
         <v>108</v>
@@ -4281,7 +4281,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="10">
-        <v>5600</v>
+        <v>4200</v>
       </c>
       <c r="C8" s="10">
         <v>134</v>
@@ -4306,7 +4306,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="10">
-        <v>7200</v>
+        <v>5600</v>
       </c>
       <c r="C9" s="10">
         <v>162</v>
@@ -4331,7 +4331,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="10">
-        <v>9000</v>
+        <v>7200</v>
       </c>
       <c r="C10" s="10">
         <v>194</v>
@@ -4356,7 +4356,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="10">
-        <v>11000</v>
+        <v>9000</v>
       </c>
       <c r="C11" s="10">
         <v>228</v>
@@ -4381,7 +4381,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="10">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="C12" s="10">
         <v>264</v>
@@ -4406,7 +4406,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10">
-        <v>15600</v>
+        <v>13200</v>
       </c>
       <c r="C13" s="10">
         <v>302</v>
@@ -4426,6 +4426,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -4443,7 +4444,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5167,7 +5168,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
bluprints moved to player
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="193">
   <si>
     <t>Class</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>thief +2</t>
+  </si>
+  <si>
+    <t>MagicSlots</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -4055,22 +4058,24 @@
         <v>162</v>
       </c>
       <c r="B85" s="1">
-        <v>1</v>
-      </c>
-      <c r="C85" s="1">
-        <v>1</v>
-      </c>
-      <c r="D85" s="1">
-        <v>1</v>
-      </c>
-      <c r="E85" s="1">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C85" s="5">
+        <v>3</v>
+      </c>
+      <c r="D85" s="5">
+        <v>1</v>
+      </c>
+      <c r="E85" s="5">
+        <f t="shared" ref="E85" si="7">C85+D85</f>
+        <v>4</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G85" s="1">
-        <v>1300</v>
+      <c r="G85" s="5">
+        <f>VLOOKUP(E85, cost!$A$3:$G$15, 3, FALSE)</f>
+        <v>3100</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>175</v>
@@ -4444,7 +4449,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4905,20 +4910,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" style="1" customWidth="1"/>
-    <col min="2" max="6" width="14.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="1.77734375" customWidth="1"/>
+    <col min="2" max="7" width="14.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -4937,8 +4942,11 @@
       <c r="F1" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4958,8 +4966,12 @@
       <c r="F2" s="10">
         <v>450</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -4973,8 +4985,8 @@
         <v>2</v>
       </c>
       <c r="D3" s="10">
-        <f>D2+0.5</f>
-        <v>6.5</v>
+        <f>D2+1</f>
+        <v>7</v>
       </c>
       <c r="E3" s="10">
         <f t="shared" ref="E3:E10" si="1">E2 +400</f>
@@ -4983,8 +4995,12 @@
       <c r="F3" s="10">
         <v>620</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A10" si="2">A3+1</f>
         <v>3</v>
@@ -4998,8 +5014,8 @@
         <v>3</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ref="D4:D10" si="4">D3+0.5</f>
-        <v>7</v>
+        <f t="shared" ref="D4:D10" si="4">D3+1</f>
+        <v>8</v>
       </c>
       <c r="E4" s="10">
         <f t="shared" si="1"/>
@@ -5008,8 +5024,12 @@
       <c r="F4" s="10">
         <v>810</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -5023,7 +5043,7 @@
       </c>
       <c r="D5" s="10">
         <f t="shared" si="4"/>
-        <v>7.5</v>
+        <v>9</v>
       </c>
       <c r="E5" s="10">
         <f t="shared" si="1"/>
@@ -5032,8 +5052,12 @@
       <c r="F5" s="10">
         <v>1100</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -5048,7 +5072,7 @@
       </c>
       <c r="D6" s="10">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" si="1"/>
@@ -5057,8 +5081,12 @@
       <c r="F6" s="10">
         <v>1400</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -5073,7 +5101,7 @@
       </c>
       <c r="D7" s="10">
         <f t="shared" si="4"/>
-        <v>8.5</v>
+        <v>11</v>
       </c>
       <c r="E7" s="10">
         <f t="shared" si="1"/>
@@ -5082,8 +5110,12 @@
       <c r="F7" s="10">
         <v>1700</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -5097,7 +5129,7 @@
       </c>
       <c r="D8" s="10">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E8" s="10">
         <f t="shared" si="1"/>
@@ -5106,8 +5138,12 @@
       <c r="F8" s="10">
         <v>2000</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -5122,7 +5158,7 @@
       </c>
       <c r="D9" s="10">
         <f t="shared" si="4"/>
-        <v>9.5</v>
+        <v>13</v>
       </c>
       <c r="E9" s="10">
         <f t="shared" si="1"/>
@@ -5131,8 +5167,12 @@
       <c r="F9" s="10">
         <v>2300</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -5147,7 +5187,7 @@
       </c>
       <c r="D10" s="10">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E10" s="10">
         <f t="shared" si="1"/>
@@ -5156,6 +5196,10 @@
       <c r="F10" s="10">
         <v>2600</v>
       </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5551,8 +5595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
castle create room progress
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="196">
   <si>
     <t>Class</t>
   </si>
@@ -344,9 +344,6 @@
     <t>Throne</t>
   </si>
   <si>
-    <t>Main Hall</t>
-  </si>
-  <si>
     <t>Keep</t>
   </si>
   <si>
@@ -398,215 +395,227 @@
     <t>AllowedPlacement</t>
   </si>
   <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>R, L</t>
-  </si>
-  <si>
     <t>Increases the max storage amount for gold.</t>
   </si>
   <si>
-    <t>Increases the max storage amount for wood, stone, and iron.</t>
-  </si>
-  <si>
     <t>Train thieves here to upgrade their level.</t>
   </si>
   <si>
+    <t>Gives the guild expedition slots.</t>
+  </si>
+  <si>
+    <t>Cartographer</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>40 min</t>
+  </si>
+  <si>
+    <t>3 hr</t>
+  </si>
+  <si>
+    <t>5 hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 min </t>
+  </si>
+  <si>
+    <t>3 min</t>
+  </si>
+  <si>
+    <t>6 min</t>
+  </si>
+  <si>
+    <t>48 hr</t>
+  </si>
+  <si>
+    <t>Fence</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>max gold</t>
+  </si>
+  <si>
+    <t>max stn</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>Jeweler</t>
+  </si>
+  <si>
+    <t>Blacksmith</t>
+  </si>
+  <si>
+    <t>Artisan</t>
+  </si>
+  <si>
+    <t>Stone_Basic</t>
+  </si>
+  <si>
+    <t>Period_Basic</t>
+  </si>
+  <si>
+    <t>6 days</t>
+  </si>
+  <si>
+    <t>4 days</t>
+  </si>
+  <si>
+    <t>initial</t>
+  </si>
+  <si>
+    <t>Throne_Gold</t>
+  </si>
+  <si>
+    <t>Throne_Stone</t>
+  </si>
+  <si>
+    <t>Cloak</t>
+  </si>
+  <si>
+    <t>end 1</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>dmg 1, def 1, per 3, tra 3</t>
+  </si>
+  <si>
+    <t>att 1, def 1, sab 3, tra 3</t>
+  </si>
+  <si>
+    <t>att 1, dmg 1, sab 3, per 3</t>
+  </si>
+  <si>
+    <t>dmg 1, def 1, sab 3, tra 3</t>
+  </si>
+  <si>
+    <t>att 1, def 1, sab 3, per 3</t>
+  </si>
+  <si>
+    <t>Enchantments</t>
+  </si>
+  <si>
+    <t>agi 1, cun 1, mig 1, end 1</t>
+  </si>
+  <si>
+    <t>att 1, dmg 1, per 3, tra 3</t>
+  </si>
+  <si>
+    <t>att 1, dmg 1, def 1, sab 3, per 3, tra 3</t>
+  </si>
+  <si>
+    <t>end 2</t>
+  </si>
+  <si>
+    <t>end 3</t>
+  </si>
+  <si>
+    <t>Cartog_Slots</t>
+  </si>
+  <si>
+    <t>Cartog_Recovery</t>
+  </si>
+  <si>
+    <t>Fence_GoldBonus</t>
+  </si>
+  <si>
+    <t>Fence_MagicSlots</t>
+  </si>
+  <si>
+    <t>Workshop_StoneBonus</t>
+  </si>
+  <si>
+    <t>Workshop_Defense</t>
+  </si>
+  <si>
+    <t>trap +1</t>
+  </si>
+  <si>
+    <t>thief +1</t>
+  </si>
+  <si>
+    <t>Jeweler_GemBonus</t>
+  </si>
+  <si>
+    <t>Jeweler_ExpedSlots</t>
+  </si>
+  <si>
+    <t>Artisan_Cost</t>
+  </si>
+  <si>
+    <t>Artisan_Period</t>
+  </si>
+  <si>
+    <t>Blacksmith_Period</t>
+  </si>
+  <si>
+    <t>20 hr</t>
+  </si>
+  <si>
+    <t>trap +2</t>
+  </si>
+  <si>
+    <t>thief +2</t>
+  </si>
+  <si>
+    <t>MagicSlots</t>
+  </si>
+  <si>
+    <t>M 1</t>
+  </si>
+  <si>
+    <t>M 2</t>
+  </si>
+  <si>
+    <t>M 3</t>
+  </si>
+  <si>
+    <t>L1, R1, R2</t>
+  </si>
+  <si>
     <t>Increases the number of thieves allowed in the guild.
-Also reduces the thieves' recovery time from wounds.</t>
-  </si>
-  <si>
-    <t>Gives the guild expedition slots.</t>
-  </si>
-  <si>
-    <t>Cartographer</t>
-  </si>
-  <si>
-    <t>20 min</t>
-  </si>
-  <si>
-    <t>40 min</t>
-  </si>
-  <si>
-    <t>3 hr</t>
-  </si>
-  <si>
-    <t>5 hr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 min </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 min </t>
-  </si>
-  <si>
-    <t>3 min</t>
-  </si>
-  <si>
-    <t>6 min</t>
-  </si>
-  <si>
-    <t>48 hr</t>
-  </si>
-  <si>
-    <t>Fence</t>
-  </si>
-  <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>max gold</t>
-  </si>
-  <si>
-    <t>max stn</t>
-  </si>
-  <si>
-    <t>Workshop</t>
-  </si>
-  <si>
-    <t>Jeweler</t>
-  </si>
-  <si>
-    <t>Blacksmith</t>
-  </si>
-  <si>
-    <t>Artisan</t>
-  </si>
-  <si>
-    <t>Stone_Basic</t>
-  </si>
-  <si>
-    <t>Stone_Throne</t>
-  </si>
-  <si>
-    <t>Stone_Advan</t>
-  </si>
-  <si>
-    <t>Period_Basic</t>
-  </si>
-  <si>
-    <t>Period_Advan</t>
-  </si>
-  <si>
-    <t>Period_Throne</t>
-  </si>
-  <si>
-    <t>6 days</t>
-  </si>
-  <si>
-    <t>4 days</t>
-  </si>
-  <si>
-    <t>4 min</t>
-  </si>
-  <si>
-    <t>initial</t>
-  </si>
-  <si>
-    <t>Throne_Gold</t>
-  </si>
-  <si>
-    <t>Throne_Stone</t>
-  </si>
-  <si>
-    <t>Cloak</t>
-  </si>
-  <si>
-    <t>end 1</t>
-  </si>
-  <si>
-    <t>back</t>
-  </si>
-  <si>
-    <t>dmg 1, def 1, per 3, tra 3</t>
-  </si>
-  <si>
-    <t>att 1, def 1, sab 3, tra 3</t>
-  </si>
-  <si>
-    <t>att 1, dmg 1, sab 3, per 3</t>
-  </si>
-  <si>
-    <t>dmg 1, def 1, sab 3, tra 3</t>
-  </si>
-  <si>
-    <t>att 1, def 1, sab 3, per 3</t>
-  </si>
-  <si>
-    <t>Enchantments</t>
-  </si>
-  <si>
-    <t>agi 1, cun 1, mig 1, end 1</t>
-  </si>
-  <si>
-    <t>att 1, dmg 1, per 3, tra 3</t>
-  </si>
-  <si>
-    <t>att 1, dmg 1, def 1, sab 3, per 3, tra 3</t>
-  </si>
-  <si>
-    <t>end 2</t>
-  </si>
-  <si>
-    <t>end 3</t>
-  </si>
-  <si>
-    <t>Cartog_Slots</t>
-  </si>
-  <si>
-    <t>Cartog_Recovery</t>
-  </si>
-  <si>
-    <t>Fence_GoldBonus</t>
-  </si>
-  <si>
-    <t>Fence_MagicSlots</t>
-  </si>
-  <si>
-    <t>Workshop_StoneBonus</t>
-  </si>
-  <si>
-    <t>Workshop_Defense</t>
-  </si>
-  <si>
-    <t>trap +1</t>
-  </si>
-  <si>
-    <t>thief +1</t>
-  </si>
-  <si>
-    <t>Jeweler_GemBonus</t>
-  </si>
-  <si>
-    <t>Jeweler_ExpedSlots</t>
-  </si>
-  <si>
-    <t>Artisan_Cost</t>
-  </si>
-  <si>
-    <t>Artisan_Period</t>
-  </si>
-  <si>
-    <t>Blacksmith_Period</t>
-  </si>
-  <si>
-    <t>20 hr</t>
-  </si>
-  <si>
-    <t>trap +2</t>
-  </si>
-  <si>
-    <t>thief +2</t>
-  </si>
-  <si>
-    <t>MagicSlots</t>
+Reduces the thieves' recovery time from wounds.</t>
+  </si>
+  <si>
+    <t>Great Hall</t>
+  </si>
+  <si>
+    <t>Increases the max storage amount for wood and stone.</t>
+  </si>
+  <si>
+    <t>Stone_Unique</t>
+  </si>
+  <si>
+    <t>Period_Unique</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>advanced</t>
+  </si>
+  <si>
+    <t>Stone_Advanced</t>
+  </si>
+  <si>
+    <t>Period_Advanced</t>
+  </si>
+  <si>
+    <t>UpgradeType</t>
   </si>
 </sst>
 </file>
@@ -1028,17 +1037,17 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1540,7 +1549,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1936,7 +1945,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1952,14 +1961,14 @@
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G15" s="5">
         <f>VLOOKUP(E15, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1996,7 +2005,7 @@
         <v>42</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2033,7 +2042,7 @@
         <v>44</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2071,7 +2080,7 @@
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2108,7 +2117,7 @@
         <v>43</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2145,7 +2154,7 @@
         <v>45</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2182,7 +2191,7 @@
         <v>46</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2213,7 +2222,7 @@
         <v>98</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2244,7 +2253,7 @@
         <v>99</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2275,7 +2284,7 @@
         <v>100</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2306,7 +2315,7 @@
         <v>46</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2337,7 +2346,7 @@
         <v>42</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2368,12 +2377,12 @@
         <v>48</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2389,17 +2398,17 @@
         <v>2</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G29" s="5">
         <f>VLOOKUP(E29, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2777,7 +2786,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B43" s="1">
         <v>2</v>
@@ -2793,14 +2802,14 @@
         <v>2</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G43" s="5">
         <f>VLOOKUP(E43, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2837,7 +2846,7 @@
         <v>42</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2874,7 +2883,7 @@
         <v>44</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -2912,7 +2921,7 @@
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -2949,7 +2958,7 @@
         <v>43</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -2986,7 +2995,7 @@
         <v>45</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -3023,7 +3032,7 @@
         <v>46</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -3054,7 +3063,7 @@
         <v>101</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -3085,7 +3094,7 @@
         <v>102</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -3116,7 +3125,7 @@
         <v>103</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -3147,7 +3156,7 @@
         <v>45</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -3178,7 +3187,7 @@
         <v>52</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -3209,12 +3218,12 @@
         <v>44</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B57" s="1">
         <v>2</v>
@@ -3230,17 +3239,17 @@
         <v>3</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G57" s="5">
         <f>VLOOKUP(E57, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3618,7 +3627,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B71" s="1">
         <v>3</v>
@@ -3634,14 +3643,14 @@
         <v>3</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G71" s="5">
         <f>VLOOKUP(E71, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -3678,7 +3687,7 @@
         <v>42</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -3715,7 +3724,7 @@
         <v>44</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -3753,7 +3762,7 @@
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -3790,7 +3799,7 @@
         <v>43</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -3827,7 +3836,7 @@
         <v>45</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -3864,7 +3873,7 @@
         <v>46</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -3895,7 +3904,7 @@
         <v>53</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -3926,7 +3935,7 @@
         <v>54</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -3957,7 +3966,7 @@
         <v>55</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -3988,7 +3997,7 @@
         <v>43</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
@@ -4019,7 +4028,7 @@
         <v>59</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
@@ -4050,12 +4059,12 @@
         <v>47</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B85" s="1">
         <v>3</v>
@@ -4071,17 +4080,17 @@
         <v>4</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G85" s="5">
         <f>VLOOKUP(E85, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4094,7 +4103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
@@ -4152,7 +4161,7 @@
         <v>83</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4177,7 +4186,7 @@
         <v>61</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -4196,10 +4205,10 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>63</v>
@@ -4224,7 +4233,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>64</v>
@@ -4421,7 +4430,7 @@
         <v>290</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>15</v>
@@ -4445,202 +4454,252 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.77734375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="64.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.77734375" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="20"/>
+    <col min="2" max="2" width="12.77734375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="64.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.77734375" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="19">
+        <v>1</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="19">
+        <v>3</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="19">
-        <v>1</v>
-      </c>
-      <c r="C2" s="19" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="19">
-        <v>1</v>
-      </c>
-      <c r="C3" s="19" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="19">
+        <v>2</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="19">
-        <v>3</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="19">
-        <v>1</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="19">
-        <v>1</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="19">
-        <v>1</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="19">
-        <v>2</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="19">
-        <v>2</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="19">
+        <v>4</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="19">
+        <v>4</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="19">
+        <v>4</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" s="19">
+        <v>4</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B12" s="19">
-        <v>4</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" s="19">
-        <v>4</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" s="19">
-        <v>4</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="19">
-        <v>4</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="19">
-        <v>4</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>126</v>
+      <c r="B17" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" s="19">
+        <v>4</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -4653,14 +4712,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" style="1" customWidth="1"/>
-    <col min="2" max="7" width="14.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="14.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" style="1" customWidth="1"/>
     <col min="8" max="8" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4669,22 +4732,22 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4707,7 +4770,7 @@
         <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4728,10 +4791,10 @@
         <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -4827,7 +4890,7 @@
         <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -4848,7 +4911,7 @@
         <v>76</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>77</v>
@@ -4869,13 +4932,13 @@
         <v>5900</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -4896,7 +4959,7 @@
         <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>78</v>
@@ -4937,13 +5000,13 @@
         <v>81</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -5232,31 +5295,31 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -5385,7 +5448,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
@@ -5419,13 +5482,13 @@
         <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="I6" s="1">
         <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -5521,7 +5584,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I9" s="1">
         <v>3</v>
@@ -5555,13 +5618,13 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="I10" s="1">
         <v>3</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -5616,31 +5679,31 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -5690,7 +5753,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F3" s="14">
         <v>1</v>
@@ -5760,7 +5823,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F5" s="14">
         <v>2</v>
@@ -5803,7 +5866,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="I6" s="10">
         <f xml:space="preserve"> cost!C8 - cost!C7</f>
@@ -5830,7 +5893,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="F7" s="14">
         <v>2</v>
@@ -5846,7 +5909,7 @@
         <v>1300</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -5900,7 +5963,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F9" s="14">
         <v>3</v>
@@ -5943,7 +6006,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="I10" s="10">
         <f xml:space="preserve"> cost!C12 - cost!C11</f>

</xml_diff>

<commit_message>
some throne traits moved to great hall
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="ThiefLevel" sheetId="4" r:id="rId4"/>
     <sheet name="CastleRoom" sheetId="9" r:id="rId5"/>
     <sheet name="RoomUpgrade" sheetId="11" r:id="rId6"/>
-    <sheet name="ThroneRoom" sheetId="3" r:id="rId7"/>
+    <sheet name="UniqueRoom" sheetId="3" r:id="rId7"/>
     <sheet name="BasicRoom" sheetId="10" r:id="rId8"/>
     <sheet name="AdvancedRoom" sheetId="8" r:id="rId9"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="197">
   <si>
     <t>Class</t>
   </si>
@@ -272,9 +272,6 @@
     <t>MaxRoomLevel</t>
   </si>
   <si>
-    <t>MaxThieves</t>
-  </si>
-  <si>
     <t>MaxRoomCount</t>
   </si>
   <si>
@@ -398,9 +395,6 @@
     <t>Increases the max storage amount for gold.</t>
   </si>
   <si>
-    <t>Train thieves here to upgrade their level.</t>
-  </si>
-  <si>
     <t>Gives the guild expedition slots.</t>
   </si>
   <si>
@@ -567,9 +561,6 @@
   </si>
   <si>
     <t>thief +2</t>
-  </si>
-  <si>
-    <t>MagicSlots</t>
   </si>
   <si>
     <t>M 1</t>
@@ -616,6 +607,18 @@
   </si>
   <si>
     <t>UpgradeType</t>
+  </si>
+  <si>
+    <t>Train thieves here to level them up.</t>
+  </si>
+  <si>
+    <t>Hall_MaxThieves</t>
+  </si>
+  <si>
+    <t>Hall_MagicStore</t>
+  </si>
+  <si>
+    <t>Hall_Expedition</t>
   </si>
 </sst>
 </file>
@@ -1037,17 +1040,17 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1224,13 +1227,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -1314,7 +1317,7 @@
         <v>6700</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -1335,7 +1338,7 @@
         <v>6700</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -1356,7 +1359,7 @@
         <v>6700</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -1377,7 +1380,7 @@
         <v>11400</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
@@ -1398,7 +1401,7 @@
         <v>11400</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
@@ -1419,7 +1422,7 @@
         <v>11400</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="1">
         <v>4</v>
@@ -1440,7 +1443,7 @@
         <v>17100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" s="1">
         <v>6</v>
@@ -1461,7 +1464,7 @@
         <v>17100</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="1">
         <v>6</v>
@@ -1482,7 +1485,7 @@
         <v>17100</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F13" s="1">
         <v>6</v>
@@ -1519,16 +1522,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>24</v>
@@ -1549,7 +1552,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1800,7 +1803,7 @@
         <v>600</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1828,7 +1831,7 @@
         <v>600</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1856,7 +1859,7 @@
         <v>600</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1889,7 +1892,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1945,7 +1948,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1961,14 +1964,14 @@
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G15" s="5">
         <f>VLOOKUP(E15, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2005,7 +2008,7 @@
         <v>42</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2042,7 +2045,7 @@
         <v>44</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2080,7 +2083,7 @@
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2117,7 +2120,7 @@
         <v>43</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2154,7 +2157,7 @@
         <v>45</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2191,7 +2194,7 @@
         <v>46</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2219,10 +2222,10 @@
         <v>1300</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2250,10 +2253,10 @@
         <v>1300</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2281,10 +2284,10 @@
         <v>1300</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2315,12 +2318,12 @@
         <v>46</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -2346,7 +2349,7 @@
         <v>42</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2377,12 +2380,12 @@
         <v>48</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2398,17 +2401,17 @@
         <v>2</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G29" s="5">
         <f>VLOOKUP(E29, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2641,7 +2644,7 @@
         <v>1300</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2669,7 +2672,7 @@
         <v>1300</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2697,7 +2700,7 @@
         <v>1300</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -2730,7 +2733,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B41" s="1">
         <v>2</v>
@@ -2786,7 +2789,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B43" s="1">
         <v>2</v>
@@ -2802,14 +2805,14 @@
         <v>2</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G43" s="5">
         <f>VLOOKUP(E43, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2846,7 +2849,7 @@
         <v>42</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2883,7 +2886,7 @@
         <v>44</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -2921,7 +2924,7 @@
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -2958,7 +2961,7 @@
         <v>43</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -2995,7 +2998,7 @@
         <v>45</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -3032,7 +3035,7 @@
         <v>46</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -3060,10 +3063,10 @@
         <v>2100</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -3091,10 +3094,10 @@
         <v>2100</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -3122,10 +3125,10 @@
         <v>2100</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -3156,12 +3159,12 @@
         <v>45</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B55" s="1">
         <v>2</v>
@@ -3187,7 +3190,7 @@
         <v>52</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -3218,12 +3221,12 @@
         <v>44</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B57" s="1">
         <v>2</v>
@@ -3239,17 +3242,17 @@
         <v>3</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G57" s="5">
         <f>VLOOKUP(E57, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3571,7 +3574,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B69" s="1">
         <v>3</v>
@@ -3627,7 +3630,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B71" s="1">
         <v>3</v>
@@ -3643,14 +3646,14 @@
         <v>3</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G71" s="5">
         <f>VLOOKUP(E71, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -3687,7 +3690,7 @@
         <v>42</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -3724,7 +3727,7 @@
         <v>44</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -3762,7 +3765,7 @@
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -3799,7 +3802,7 @@
         <v>43</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -3836,7 +3839,7 @@
         <v>45</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -3873,7 +3876,7 @@
         <v>46</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -3904,7 +3907,7 @@
         <v>53</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -3935,7 +3938,7 @@
         <v>54</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -3966,7 +3969,7 @@
         <v>55</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -3997,12 +4000,12 @@
         <v>43</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B83" s="1">
         <v>3</v>
@@ -4028,7 +4031,7 @@
         <v>59</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
@@ -4059,12 +4062,12 @@
         <v>47</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B85" s="1">
         <v>3</v>
@@ -4080,17 +4083,17 @@
         <v>4</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G85" s="5">
         <f>VLOOKUP(E85, cost!$A$3:$G$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -4158,10 +4161,10 @@
         <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4186,7 +4189,7 @@
         <v>61</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -4205,10 +4208,10 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>63</v>
@@ -4233,7 +4236,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>64</v>
@@ -4430,7 +4433,7 @@
         <v>290</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>15</v>
@@ -4458,7 +4461,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4477,16 +4480,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -4498,208 +4501,208 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C3" s="19">
         <v>1</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C4" s="19">
         <v>1</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C5" s="19">
         <v>3</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C7" s="19">
         <v>1</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
       </c>
       <c r="D8" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>184</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>123</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C10" s="19">
         <v>2</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C11" s="19">
         <v>2</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C13" s="19">
         <v>4</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C14" s="19">
         <v>4</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C15" s="19">
         <v>4</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C16" s="19">
         <v>4</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C17" s="19">
         <v>4</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4712,7 +4715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -4732,22 +4735,22 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4770,7 +4773,7 @@
         <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4791,7 +4794,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>62</v>
@@ -4890,7 +4893,7 @@
         <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -4911,7 +4914,7 @@
         <v>76</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>77</v>
@@ -4932,13 +4935,13 @@
         <v>5900</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -4959,7 +4962,7 @@
         <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>78</v>
@@ -4973,43 +4976,53 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" style="1" customWidth="1"/>
-    <col min="2" max="7" width="14.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="1.77734375" customWidth="1"/>
+    <col min="2" max="8" width="14.77734375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="14.77734375" customWidth="1"/>
+    <col min="11" max="11" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5021,20 +5034,29 @@
         <v>1</v>
       </c>
       <c r="D2" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="10">
+        <v>450</v>
+      </c>
+      <c r="F2" s="10">
         <v>6</v>
       </c>
-      <c r="E2" s="10">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="10">
-        <v>450</v>
-      </c>
       <c r="G2" s="10">
+        <v>4</v>
+      </c>
+      <c r="H2" s="10">
         <v>0</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -5048,22 +5070,31 @@
         <v>2</v>
       </c>
       <c r="D3" s="10">
-        <f>D2+1</f>
+        <f t="shared" ref="D3:D10" si="1">D2 +400</f>
+        <v>1400</v>
+      </c>
+      <c r="E3" s="10">
+        <v>620</v>
+      </c>
+      <c r="F3" s="10">
+        <f>F2+1</f>
         <v>7</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" ref="E3:E10" si="1">E2 +400</f>
-        <v>1400</v>
-      </c>
-      <c r="F3" s="10">
-        <v>620</v>
-      </c>
       <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A10" si="2">A3+1</f>
         <v>3</v>
@@ -5077,22 +5108,31 @@
         <v>3</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ref="D4:D10" si="4">D3+1</f>
-        <v>8</v>
-      </c>
-      <c r="E4" s="10">
         <f t="shared" si="1"/>
         <v>1800</v>
       </c>
+      <c r="E4" s="10">
+        <v>810</v>
+      </c>
       <c r="F4" s="10">
-        <v>810</v>
+        <f t="shared" ref="F4:F10" si="4">F3+1</f>
+        <v>8</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -5105,22 +5145,31 @@
         <v>4</v>
       </c>
       <c r="D5" s="10">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1100</v>
+      </c>
+      <c r="F5" s="10">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="E5" s="10">
-        <f t="shared" si="1"/>
-        <v>2200</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1100</v>
-      </c>
       <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -5134,22 +5183,31 @@
         <v>5</v>
       </c>
       <c r="D6" s="10">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1400</v>
+      </c>
+      <c r="F6" s="10">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="1"/>
-        <v>2600</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1400</v>
-      </c>
       <c r="G6" s="1">
-        <v>2</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -5163,22 +5221,31 @@
         <v>6</v>
       </c>
       <c r="D7" s="10">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1700</v>
+      </c>
+      <c r="F7" s="10">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1700</v>
-      </c>
       <c r="G7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -5191,22 +5258,31 @@
         <v>7</v>
       </c>
       <c r="D8" s="10">
+        <f t="shared" si="1"/>
+        <v>3400</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F8" s="10">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="E8" s="10">
-        <f t="shared" si="1"/>
-        <v>3400</v>
-      </c>
-      <c r="F8" s="10">
-        <v>2000</v>
-      </c>
       <c r="G8" s="1">
-        <v>3</v>
-      </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -5220,22 +5296,31 @@
         <v>8</v>
       </c>
       <c r="D9" s="10">
+        <f t="shared" si="1"/>
+        <v>3800</v>
+      </c>
+      <c r="E9" s="10">
+        <v>2300</v>
+      </c>
+      <c r="F9" s="10">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="E9" s="10">
-        <f t="shared" si="1"/>
-        <v>3800</v>
-      </c>
-      <c r="F9" s="10">
-        <v>2300</v>
-      </c>
       <c r="G9" s="1">
-        <v>3</v>
-      </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -5249,20 +5334,29 @@
         <v>9</v>
       </c>
       <c r="D10" s="10">
+        <f t="shared" si="1"/>
+        <v>4200</v>
+      </c>
+      <c r="E10" s="10">
+        <v>2600</v>
+      </c>
+      <c r="F10" s="10">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="E10" s="10">
-        <f t="shared" si="1"/>
-        <v>4200</v>
-      </c>
-      <c r="F10" s="10">
-        <v>2600</v>
-      </c>
       <c r="G10" s="1">
-        <v>4</v>
-      </c>
-      <c r="I10" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4</v>
+      </c>
+      <c r="J10" s="1">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5272,381 +5366,321 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="11">
-        <v>0</v>
-      </c>
-      <c r="D2" s="10">
+      <c r="B2" s="10">
         <v>1200</v>
       </c>
-      <c r="E2" s="10">
+      <c r="C2" s="10">
         <v>310</v>
       </c>
-      <c r="F2" s="1">
+      <c r="D2" s="1">
         <f>A2+3</f>
         <v>4</v>
       </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="11">
-        <v>1</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="B3" s="10">
         <v>2300</v>
       </c>
-      <c r="E3" s="10">
+      <c r="C3" s="10">
         <v>650</v>
       </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F10" si="0">A3+3</f>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D10" si="0">A3+3</f>
         <v>5</v>
       </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A10" si="1">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="B4" s="10">
         <v>3700</v>
       </c>
-      <c r="E4" s="10">
+      <c r="C4" s="10">
         <v>1000</v>
       </c>
-      <c r="F4" s="1">
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="G4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="B5" s="10">
         <v>5200</v>
       </c>
-      <c r="E5" s="10">
+      <c r="C5" s="10">
         <v>1400</v>
       </c>
-      <c r="F5" s="1">
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="G5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="B6" s="10">
         <v>6300</v>
       </c>
-      <c r="E6" s="10">
+      <c r="C6" s="10">
         <v>1900</v>
       </c>
-      <c r="F6" s="1">
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="G6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" s="1">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="B7" s="10">
         <v>8500</v>
       </c>
-      <c r="E7" s="10">
+      <c r="C7" s="10">
         <v>2500</v>
       </c>
-      <c r="F7" s="1">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="B8" s="10">
         <v>10800</v>
       </c>
-      <c r="E8" s="10">
+      <c r="C8" s="10">
         <v>3200</v>
       </c>
-      <c r="F8" s="1">
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="G8" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="1">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="B9" s="10">
         <v>12300</v>
       </c>
-      <c r="E9" s="10">
+      <c r="C9" s="10">
         <v>3900</v>
       </c>
-      <c r="F9" s="1">
+      <c r="D9" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="G9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I9" s="1">
-        <v>3</v>
-      </c>
-      <c r="J9" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4</v>
-      </c>
-      <c r="D10" s="10">
+      <c r="B10" s="10">
         <v>14000</v>
       </c>
-      <c r="E10" s="10">
+      <c r="C10" s="10">
         <v>4600</v>
       </c>
-      <c r="F10" s="1">
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="G10" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I10" s="1">
-        <v>3</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" s="1"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5659,7 +5693,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5679,31 +5713,31 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>169</v>
-      </c>
       <c r="F1" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="J1" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -5753,7 +5787,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F3" s="14">
         <v>1</v>
@@ -5823,7 +5857,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F5" s="14">
         <v>2</v>
@@ -5866,7 +5900,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I6" s="10">
         <f xml:space="preserve"> cost!C8 - cost!C7</f>
@@ -5893,7 +5927,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F7" s="14">
         <v>2</v>
@@ -5909,7 +5943,7 @@
         <v>1300</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -5963,7 +5997,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F9" s="14">
         <v>3</v>
@@ -6006,7 +6040,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I10" s="10">
         <f xml:space="preserve"> cost!C12 - cost!C11</f>

</xml_diff>

<commit_message>
room upgrade loop finished
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -5074,7 +5074,7 @@
         <v>1400</v>
       </c>
       <c r="E3" s="10">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="F3" s="10">
         <f>F2+1</f>
@@ -5112,7 +5112,7 @@
         <v>1800</v>
       </c>
       <c r="E4" s="10">
-        <v>810</v>
+        <v>750</v>
       </c>
       <c r="F4" s="10">
         <f t="shared" ref="F4:F10" si="4">F3+1</f>
@@ -5149,7 +5149,7 @@
         <v>2200</v>
       </c>
       <c r="E5" s="10">
-        <v>1100</v>
+        <v>900</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" si="4"/>
@@ -5187,7 +5187,7 @@
         <v>2600</v>
       </c>
       <c r="E6" s="10">
-        <v>1400</v>
+        <v>1100</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="4"/>
@@ -5224,8 +5224,8 @@
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="E7" s="10">
-        <v>1700</v>
+      <c r="E7" s="1">
+        <v>1300</v>
       </c>
       <c r="F7" s="10">
         <f t="shared" si="4"/>
@@ -5261,8 +5261,8 @@
         <f t="shared" si="1"/>
         <v>3400</v>
       </c>
-      <c r="E8" s="10">
-        <v>2000</v>
+      <c r="E8" s="1">
+        <v>1500</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="4"/>
@@ -5299,8 +5299,8 @@
         <f t="shared" si="1"/>
         <v>3800</v>
       </c>
-      <c r="E9" s="10">
-        <v>2300</v>
+      <c r="E9" s="1">
+        <v>1750</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="4"/>
@@ -5337,8 +5337,8 @@
         <f t="shared" si="1"/>
         <v>4200</v>
       </c>
-      <c r="E10" s="10">
-        <v>2600</v>
+      <c r="E10" s="1">
+        <v>2000</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="4"/>
@@ -5366,7 +5366,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -5376,7 +5376,7 @@
   <cols>
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14.77734375" style="1" customWidth="1"/>
@@ -5418,7 +5418,7 @@
         <v>1200</v>
       </c>
       <c r="C2" s="10">
-        <v>310</v>
+        <v>800</v>
       </c>
       <c r="D2" s="1">
         <f>A2+3</f>
@@ -5446,7 +5446,7 @@
         <v>2300</v>
       </c>
       <c r="C3" s="10">
-        <v>650</v>
+        <v>1250</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D10" si="0">A3+3</f>
@@ -5474,7 +5474,7 @@
         <v>3700</v>
       </c>
       <c r="C4" s="10">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
@@ -5502,7 +5502,7 @@
         <v>5200</v>
       </c>
       <c r="C5" s="10">
-        <v>1400</v>
+        <v>2400</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
@@ -5530,7 +5530,7 @@
         <v>6300</v>
       </c>
       <c r="C6" s="10">
-        <v>1900</v>
+        <v>3100</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
@@ -5557,8 +5557,8 @@
       <c r="B7" s="10">
         <v>8500</v>
       </c>
-      <c r="C7" s="10">
-        <v>2500</v>
+      <c r="C7" s="1">
+        <v>3900</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
@@ -5585,8 +5585,8 @@
       <c r="B8" s="10">
         <v>10800</v>
       </c>
-      <c r="C8" s="10">
-        <v>3200</v>
+      <c r="C8" s="1">
+        <v>4700</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
@@ -5613,8 +5613,8 @@
       <c r="B9" s="10">
         <v>12300</v>
       </c>
-      <c r="C9" s="10">
-        <v>3900</v>
+      <c r="C9" s="1">
+        <v>5500</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
@@ -5641,8 +5641,8 @@
       <c r="B10" s="10">
         <v>14000</v>
       </c>
-      <c r="C10" s="10">
-        <v>4600</v>
+      <c r="C10" s="1">
+        <v>6400</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
@@ -5661,26 +5661,14 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-    </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
-    </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-    </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
heists and combat rebalanced
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
@@ -1501,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -5368,7 +5368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
git version reset and guild selection bug fix
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
@@ -1501,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -5368,7 +5368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
campaign world advancement implemented
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="828" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" tabRatio="828" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="195">
   <si>
     <t>Class</t>
   </si>
@@ -317,9 +317,6 @@
     <t>Gauntlet</t>
   </si>
   <si>
-    <t>UnlockThrone</t>
-  </si>
-  <si>
     <t>per 3</t>
   </si>
   <si>
@@ -432,12 +429,6 @@
   </si>
   <si>
     <t>gold</t>
-  </si>
-  <si>
-    <t>max gold</t>
-  </si>
-  <si>
-    <t>max stn</t>
   </si>
   <si>
     <t>Workshop</t>
@@ -619,6 +610,9 @@
   </si>
   <si>
     <t>Hall_Expedition</t>
+  </si>
+  <si>
+    <t>UnlockLevel</t>
   </si>
 </sst>
 </file>
@@ -1016,11 +1010,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,44 +1023,32 @@
     <col min="2" max="2" width="1.77734375" style="1" customWidth="1"/>
     <col min="3" max="4" width="10.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="1.77734375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="1.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1075,7 +1057,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>A3+1</f>
         <v>2</v>
@@ -1085,7 +1067,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f t="shared" ref="A5:A15" si="0">A4+1</f>
         <v>3</v>
@@ -1095,7 +1077,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1105,7 +1087,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1115,7 +1097,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1125,7 +1107,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1135,7 +1117,7 @@
         <v>6700</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1145,7 +1127,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1155,7 +1137,7 @@
         <v>9700</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1164,7 +1146,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1173,7 +1155,7 @@
         <v>13200</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1182,7 +1164,7 @@
         <v>15100</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1191,7 +1173,7 @@
         <v>17100</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" s="10"/>
     </row>
   </sheetData>
@@ -1227,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>194</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
@@ -1501,15 +1483,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="5" width="8.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.77734375" style="1" customWidth="1"/>
     <col min="6" max="7" width="10.77734375" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.77734375" style="8" customWidth="1"/>
     <col min="9" max="11" width="10.77734375" style="1" customWidth="1"/>
@@ -1522,7 +1505,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
@@ -1552,7 +1535,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1588,7 +1571,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="5">
-        <f>VLOOKUP(E3, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E3, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -1623,7 +1606,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="5">
-        <f>VLOOKUP(E4, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E4, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="H4" s="8" t="s">
@@ -1658,7 +1641,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="5">
-        <f>VLOOKUP(E5, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E5, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="H5" t="s">
@@ -1694,7 +1677,7 @@
         <v>26</v>
       </c>
       <c r="G6" s="5">
-        <f>VLOOKUP(E6, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E6, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="H6" s="8" t="s">
@@ -1729,7 +1712,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="5">
-        <f>VLOOKUP(E7, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E7, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -1764,7 +1747,7 @@
         <v>26</v>
       </c>
       <c r="G8" s="5">
-        <f>VLOOKUP(E8, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E8, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="H8" t="s">
@@ -1799,11 +1782,11 @@
         <v>27</v>
       </c>
       <c r="G9" s="5">
-        <f>VLOOKUP(E9, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E9, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1827,11 +1810,11 @@
         <v>28</v>
       </c>
       <c r="G10" s="5">
-        <f>VLOOKUP(E10, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E10, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1855,11 +1838,11 @@
         <v>29</v>
       </c>
       <c r="G11" s="5">
-        <f>VLOOKUP(E11, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E11, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1883,7 +1866,7 @@
         <v>27</v>
       </c>
       <c r="G12" s="5">
-        <f>VLOOKUP(E12, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E12, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1911,7 +1894,7 @@
         <v>28</v>
       </c>
       <c r="G13" s="5">
-        <f>VLOOKUP(E13, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E13, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -1939,7 +1922,7 @@
         <v>29</v>
       </c>
       <c r="G14" s="5">
-        <f>VLOOKUP(E14, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E14, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -1948,7 +1931,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1964,14 +1947,14 @@
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G15" s="5">
-        <f>VLOOKUP(E15, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E15, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1995,7 +1978,7 @@
         <v>25</v>
       </c>
       <c r="G17" s="5">
-        <f>VLOOKUP(E17, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E17, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H17" s="8" t="s">
@@ -2008,7 +1991,7 @@
         <v>42</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2032,7 +2015,7 @@
         <v>25</v>
       </c>
       <c r="G18" s="5">
-        <f>VLOOKUP(E18, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E18, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H18" s="8" t="s">
@@ -2045,7 +2028,7 @@
         <v>44</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2069,7 +2052,7 @@
         <v>25</v>
       </c>
       <c r="G19" s="5">
-        <f>VLOOKUP(E19, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E19, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H19" t="s">
@@ -2083,7 +2066,7 @@
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2107,7 +2090,7 @@
         <v>26</v>
       </c>
       <c r="G20" s="5">
-        <f>VLOOKUP(E20, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E20, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H20" s="8" t="s">
@@ -2120,7 +2103,7 @@
         <v>43</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2144,7 +2127,7 @@
         <v>26</v>
       </c>
       <c r="G21" s="5">
-        <f>VLOOKUP(E21, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E21, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H21" s="8" t="s">
@@ -2157,7 +2140,7 @@
         <v>45</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2181,7 +2164,7 @@
         <v>26</v>
       </c>
       <c r="G22" s="5">
-        <f>VLOOKUP(E22, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E22, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H22" t="s">
@@ -2194,7 +2177,7 @@
         <v>46</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2218,14 +2201,14 @@
         <v>27</v>
       </c>
       <c r="G23" s="5">
-        <f>VLOOKUP(E23, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E23, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2249,14 +2232,14 @@
         <v>28</v>
       </c>
       <c r="G24" s="5">
-        <f>VLOOKUP(E24, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E24, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2280,14 +2263,14 @@
         <v>29</v>
       </c>
       <c r="G25" s="5">
-        <f>VLOOKUP(E25, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E25, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2311,14 +2294,14 @@
         <v>27</v>
       </c>
       <c r="G26" s="5">
-        <f>VLOOKUP(E26, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E26, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>46</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2342,14 +2325,14 @@
         <v>28</v>
       </c>
       <c r="G27" s="5">
-        <f>VLOOKUP(E27, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E27, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>42</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2373,19 +2356,19 @@
         <v>29</v>
       </c>
       <c r="G28" s="5">
-        <f>VLOOKUP(E28, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E28, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>48</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2401,17 +2384,17 @@
         <v>2</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G29" s="5">
-        <f>VLOOKUP(E29, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E29, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2435,7 +2418,7 @@
         <v>25</v>
       </c>
       <c r="G31" s="5">
-        <f>VLOOKUP(E31, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E31, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H31" s="8" t="s">
@@ -2469,7 +2452,7 @@
         <v>25</v>
       </c>
       <c r="G32" s="5">
-        <f>VLOOKUP(E32, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E32, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H32" s="8" t="s">
@@ -2503,7 +2486,7 @@
         <v>25</v>
       </c>
       <c r="G33" s="5">
-        <f>VLOOKUP(E33, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E33, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H33" t="s">
@@ -2538,7 +2521,7 @@
         <v>26</v>
       </c>
       <c r="G34" s="5">
-        <f>VLOOKUP(E34, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E34, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H34" s="8" t="s">
@@ -2572,7 +2555,7 @@
         <v>26</v>
       </c>
       <c r="G35" s="5">
-        <f>VLOOKUP(E35, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E35, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H35" s="8" t="s">
@@ -2606,7 +2589,7 @@
         <v>26</v>
       </c>
       <c r="G36" s="5">
-        <f>VLOOKUP(E36, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E36, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="H36" t="s">
@@ -2640,11 +2623,11 @@
         <v>27</v>
       </c>
       <c r="G37" s="5">
-        <f>VLOOKUP(E37, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E37, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2668,11 +2651,11 @@
         <v>28</v>
       </c>
       <c r="G38" s="5">
-        <f>VLOOKUP(E38, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E38, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2696,11 +2679,11 @@
         <v>29</v>
       </c>
       <c r="G39" s="5">
-        <f>VLOOKUP(E39, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E39, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -2724,7 +2707,7 @@
         <v>27</v>
       </c>
       <c r="G40" s="5">
-        <f>VLOOKUP(E40, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E40, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="J40" s="1" t="s">
@@ -2752,7 +2735,7 @@
         <v>28</v>
       </c>
       <c r="G41" s="5">
-        <f>VLOOKUP(E41, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E41, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="J41" s="1" t="s">
@@ -2780,7 +2763,7 @@
         <v>29</v>
       </c>
       <c r="G42" s="5">
-        <f>VLOOKUP(E42, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E42, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="J42" s="1" t="s">
@@ -2789,7 +2772,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B43" s="1">
         <v>2</v>
@@ -2805,14 +2788,14 @@
         <v>2</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G43" s="5">
-        <f>VLOOKUP(E43, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E43, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2836,7 +2819,7 @@
         <v>25</v>
       </c>
       <c r="G45" s="5">
-        <f>VLOOKUP(E45, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E45, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H45" s="8" t="s">
@@ -2849,7 +2832,7 @@
         <v>42</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2873,7 +2856,7 @@
         <v>25</v>
       </c>
       <c r="G46" s="5">
-        <f>VLOOKUP(E46, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E46, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H46" s="8" t="s">
@@ -2886,7 +2869,7 @@
         <v>44</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -2910,7 +2893,7 @@
         <v>25</v>
       </c>
       <c r="G47" s="5">
-        <f>VLOOKUP(E47, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E47, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H47" t="s">
@@ -2924,7 +2907,7 @@
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -2948,7 +2931,7 @@
         <v>26</v>
       </c>
       <c r="G48" s="5">
-        <f>VLOOKUP(E48, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E48, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H48" s="8" t="s">
@@ -2961,7 +2944,7 @@
         <v>43</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -2985,7 +2968,7 @@
         <v>26</v>
       </c>
       <c r="G49" s="5">
-        <f>VLOOKUP(E49, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E49, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H49" s="8" t="s">
@@ -2998,7 +2981,7 @@
         <v>45</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -3022,7 +3005,7 @@
         <v>26</v>
       </c>
       <c r="G50" s="5">
-        <f>VLOOKUP(E50, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E50, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H50" t="s">
@@ -3035,7 +3018,7 @@
         <v>46</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -3059,14 +3042,14 @@
         <v>27</v>
       </c>
       <c r="G51" s="5">
-        <f>VLOOKUP(E51, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E51, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -3090,14 +3073,14 @@
         <v>28</v>
       </c>
       <c r="G52" s="5">
-        <f>VLOOKUP(E52, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E52, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -3121,14 +3104,14 @@
         <v>29</v>
       </c>
       <c r="G53" s="5">
-        <f>VLOOKUP(E53, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E53, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -3152,14 +3135,14 @@
         <v>27</v>
       </c>
       <c r="G54" s="5">
-        <f>VLOOKUP(E54, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E54, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -3183,14 +3166,14 @@
         <v>28</v>
       </c>
       <c r="G55" s="5">
-        <f>VLOOKUP(E55, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E55, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>52</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -3214,19 +3197,19 @@
         <v>29</v>
       </c>
       <c r="G56" s="5">
-        <f>VLOOKUP(E56, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E56, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B57" s="1">
         <v>2</v>
@@ -3242,17 +3225,17 @@
         <v>3</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G57" s="5">
-        <f>VLOOKUP(E57, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E57, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3276,7 +3259,7 @@
         <v>25</v>
       </c>
       <c r="G59" s="5">
-        <f>VLOOKUP(E59, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E59, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H59" s="8" t="s">
@@ -3310,7 +3293,7 @@
         <v>25</v>
       </c>
       <c r="G60" s="5">
-        <f>VLOOKUP(E60, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E60, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H60" s="8" t="s">
@@ -3344,7 +3327,7 @@
         <v>25</v>
       </c>
       <c r="G61" s="5">
-        <f>VLOOKUP(E61, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E61, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H61" t="s">
@@ -3379,7 +3362,7 @@
         <v>26</v>
       </c>
       <c r="G62" s="5">
-        <f>VLOOKUP(E62, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E62, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H62" s="8" t="s">
@@ -3413,7 +3396,7 @@
         <v>26</v>
       </c>
       <c r="G63" s="5">
-        <f>VLOOKUP(E63, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E63, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H63" s="8" t="s">
@@ -3447,7 +3430,7 @@
         <v>26</v>
       </c>
       <c r="G64" s="5">
-        <f>VLOOKUP(E64, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E64, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="H64" t="s">
@@ -3481,7 +3464,7 @@
         <v>27</v>
       </c>
       <c r="G65" s="5">
-        <f>VLOOKUP(E65, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E65, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="K65" s="1" t="s">
@@ -3509,7 +3492,7 @@
         <v>28</v>
       </c>
       <c r="G66" s="5">
-        <f>VLOOKUP(E66, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E66, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="K66" s="1" t="s">
@@ -3537,7 +3520,7 @@
         <v>29</v>
       </c>
       <c r="G67" s="5">
-        <f>VLOOKUP(E67, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E67, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="K67" s="1" t="s">
@@ -3565,7 +3548,7 @@
         <v>27</v>
       </c>
       <c r="G68" s="5">
-        <f>VLOOKUP(E68, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E68, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="J68" s="1" t="s">
@@ -3593,7 +3576,7 @@
         <v>28</v>
       </c>
       <c r="G69" s="5">
-        <f>VLOOKUP(E69, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E69, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="J69" s="1" t="s">
@@ -3621,7 +3604,7 @@
         <v>29</v>
       </c>
       <c r="G70" s="5">
-        <f>VLOOKUP(E70, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E70, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="J70" s="1" t="s">
@@ -3630,7 +3613,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B71" s="1">
         <v>3</v>
@@ -3646,14 +3629,14 @@
         <v>3</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G71" s="5">
-        <f>VLOOKUP(E71, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E71, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -3677,7 +3660,7 @@
         <v>25</v>
       </c>
       <c r="G73" s="5">
-        <f>VLOOKUP(E73, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E73, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>4200</v>
       </c>
       <c r="H73" s="8" t="s">
@@ -3690,7 +3673,7 @@
         <v>42</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -3714,7 +3697,7 @@
         <v>25</v>
       </c>
       <c r="G74" s="5">
-        <f>VLOOKUP(E74, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E74, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>4200</v>
       </c>
       <c r="H74" s="8" t="s">
@@ -3727,7 +3710,7 @@
         <v>44</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -3751,7 +3734,7 @@
         <v>25</v>
       </c>
       <c r="G75" s="5">
-        <f>VLOOKUP(E75, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E75, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>4200</v>
       </c>
       <c r="H75" t="s">
@@ -3765,7 +3748,7 @@
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -3789,7 +3772,7 @@
         <v>26</v>
       </c>
       <c r="G76" s="5">
-        <f>VLOOKUP(E76, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E76, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>4200</v>
       </c>
       <c r="H76" s="8" t="s">
@@ -3802,7 +3785,7 @@
         <v>43</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -3826,7 +3809,7 @@
         <v>26</v>
       </c>
       <c r="G77" s="5">
-        <f>VLOOKUP(E77, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E77, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>4200</v>
       </c>
       <c r="H77" s="8" t="s">
@@ -3839,7 +3822,7 @@
         <v>45</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -3863,7 +3846,7 @@
         <v>26</v>
       </c>
       <c r="G78" s="5">
-        <f>VLOOKUP(E78, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E78, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>4200</v>
       </c>
       <c r="H78" t="s">
@@ -3876,7 +3859,7 @@
         <v>46</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -3900,14 +3883,14 @@
         <v>27</v>
       </c>
       <c r="G79" s="5">
-        <f>VLOOKUP(E79, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E79, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>53</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -3931,14 +3914,14 @@
         <v>28</v>
       </c>
       <c r="G80" s="5">
-        <f>VLOOKUP(E80, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E80, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>54</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -3962,14 +3945,14 @@
         <v>29</v>
       </c>
       <c r="G81" s="5">
-        <f>VLOOKUP(E81, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E81, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>55</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -3993,14 +3976,14 @@
         <v>27</v>
       </c>
       <c r="G82" s="5">
-        <f>VLOOKUP(E82, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E82, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
@@ -4024,14 +4007,14 @@
         <v>28</v>
       </c>
       <c r="G83" s="5">
-        <f>VLOOKUP(E83, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E83, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>59</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
@@ -4055,19 +4038,19 @@
         <v>29</v>
       </c>
       <c r="G84" s="5">
-        <f>VLOOKUP(E84, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E84, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>47</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B85" s="1">
         <v>3</v>
@@ -4083,17 +4066,17 @@
         <v>4</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G85" s="5">
-        <f>VLOOKUP(E85, cost!$A$3:$G$15, 3, FALSE)</f>
+        <f>VLOOKUP(E85, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4164,7 +4147,7 @@
         <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4189,7 +4172,7 @@
         <v>61</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -4208,10 +4191,10 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>63</v>
@@ -4236,7 +4219,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>64</v>
@@ -4433,7 +4416,7 @@
         <v>290</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>15</v>
@@ -4461,7 +4444,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4480,16 +4463,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>96</v>
+        <v>194</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -4501,208 +4484,208 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C3" s="19">
         <v>1</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C4" s="19">
         <v>1</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C5" s="19">
         <v>3</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C7" s="19">
         <v>1</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
       </c>
       <c r="D8" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>181</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C10" s="19">
         <v>2</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C11" s="19">
         <v>2</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C13" s="19">
         <v>4</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C14" s="19">
         <v>4</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C15" s="19">
         <v>4</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C16" s="19">
         <v>4</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C17" s="19">
         <v>4</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4716,7 +4699,8 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4735,22 +4719,22 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4773,7 +4757,7 @@
         <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4794,7 +4778,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>62</v>
@@ -4893,7 +4877,7 @@
         <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -4914,7 +4898,7 @@
         <v>76</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>77</v>
@@ -4935,13 +4919,13 @@
         <v>5900</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -4962,7 +4946,7 @@
         <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>78</v>
@@ -4979,7 +4963,8 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5001,25 +4986,25 @@
         <v>80</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -5368,8 +5353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5389,25 +5375,25 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -5512,7 +5498,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -5540,13 +5526,13 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -5624,7 +5610,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G9" s="1">
         <v>3</v>
@@ -5652,13 +5638,13 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -5681,7 +5667,8 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5701,31 +5688,31 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -5775,7 +5762,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F3" s="14">
         <v>1</v>
@@ -5845,7 +5832,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F5" s="14">
         <v>2</v>
@@ -5888,7 +5875,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I6" s="10">
         <f xml:space="preserve"> cost!C8 - cost!C7</f>
@@ -5915,7 +5902,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F7" s="14">
         <v>2</v>
@@ -5931,7 +5918,7 @@
         <v>1300</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -5985,7 +5972,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F9" s="14">
         <v>3</v>
@@ -6028,7 +6015,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I10" s="10">
         <f xml:space="preserve"> cost!C12 - cost!C11</f>

</xml_diff>

<commit_message>
campaign playthrough updates progress
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" tabRatio="828" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" tabRatio="828" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
@@ -1483,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
@@ -4089,7 +4089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
@@ -4156,7 +4156,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C3" s="10">
         <v>26</v>
@@ -4181,7 +4181,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="C4" s="10">
         <v>42</v>
@@ -4206,7 +4206,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="C5" s="10">
         <v>62</v>
@@ -4231,7 +4231,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C6" s="10">
         <v>84</v>
@@ -4256,7 +4256,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10">
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="C7" s="10">
         <v>108</v>
@@ -4281,7 +4281,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="10">
-        <v>6300</v>
+        <v>4200</v>
       </c>
       <c r="C8" s="10">
         <v>134</v>
@@ -4306,7 +4306,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="10">
-        <v>8400</v>
+        <v>5600</v>
       </c>
       <c r="C9" s="10">
         <v>162</v>
@@ -4331,7 +4331,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="10">
-        <v>10800</v>
+        <v>7200</v>
       </c>
       <c r="C10" s="10">
         <v>194</v>
@@ -4356,7 +4356,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="10">
-        <v>13500</v>
+        <v>9000</v>
       </c>
       <c r="C11" s="10">
         <v>228</v>
@@ -4381,7 +4381,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="10">
-        <v>16500</v>
+        <v>11000</v>
       </c>
       <c r="C12" s="10">
         <v>264</v>
@@ -4406,7 +4406,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10">
-        <v>19800</v>
+        <v>13200</v>
       </c>
       <c r="C13" s="10">
         <v>302</v>

</xml_diff>

<commit_message>
thief recovery using dorms
</commit_message>
<xml_diff>
--- a/backend/emporium/data/GuildData.xlsx
+++ b/backend/emporium/data/GuildData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" tabRatio="828" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" tabRatio="828" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="207">
   <si>
     <t>Class</t>
   </si>
@@ -254,9 +254,6 @@
     <t>RawPower</t>
   </si>
   <si>
-    <t>KnockedOutPeriod</t>
-  </si>
-  <si>
     <t>3 days</t>
   </si>
   <si>
@@ -411,9 +408,6 @@
   </si>
   <si>
     <t>3 min</t>
-  </si>
-  <si>
-    <t>6 min</t>
   </si>
   <si>
     <t>48 hr</t>
@@ -619,6 +613,42 @@
   </si>
   <si>
     <t>27 hr</t>
+  </si>
+  <si>
+    <t>WoundPeriodMin</t>
+  </si>
+  <si>
+    <t>BeatenPeriod</t>
+  </si>
+  <si>
+    <t>BeatenPeriodMin</t>
+  </si>
+  <si>
+    <t>4 min</t>
+  </si>
+  <si>
+    <t>8 min</t>
+  </si>
+  <si>
+    <t>12 min</t>
+  </si>
+  <si>
+    <t>16 min</t>
+  </si>
+  <si>
+    <t>24 min</t>
+  </si>
+  <si>
+    <t>28 min</t>
+  </si>
+  <si>
+    <t>32 min</t>
+  </si>
+  <si>
+    <t>36 min</t>
+  </si>
+  <si>
+    <t>10 hr</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1068,10 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -1215,13 +1245,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -1305,7 +1335,7 @@
         <v>6700</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -1326,7 +1356,7 @@
         <v>6700</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -1347,7 +1377,7 @@
         <v>6700</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -1368,7 +1398,7 @@
         <v>11400</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
@@ -1389,7 +1419,7 @@
         <v>11400</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
@@ -1410,7 +1440,7 @@
         <v>11400</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="1">
         <v>4</v>
@@ -1431,7 +1461,7 @@
         <v>17100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="1">
         <v>6</v>
@@ -1452,7 +1482,7 @@
         <v>17100</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="1">
         <v>6</v>
@@ -1473,7 +1503,7 @@
         <v>17100</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="1">
         <v>6</v>
@@ -1511,16 +1541,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>24</v>
@@ -1541,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1792,7 +1822,7 @@
         <v>600</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1820,7 +1850,7 @@
         <v>600</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1848,7 +1878,7 @@
         <v>600</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1881,7 +1911,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1937,7 +1967,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1953,14 +1983,14 @@
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G15" s="5">
         <f>VLOOKUP(E15, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1997,7 +2027,7 @@
         <v>42</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2034,7 +2064,7 @@
         <v>44</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2072,7 +2102,7 @@
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2109,7 +2139,7 @@
         <v>43</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2146,7 +2176,7 @@
         <v>45</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2183,7 +2213,7 @@
         <v>46</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2211,10 +2241,10 @@
         <v>1300</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2242,10 +2272,10 @@
         <v>1300</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2273,10 +2303,10 @@
         <v>1300</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2307,12 +2337,12 @@
         <v>46</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -2338,7 +2368,7 @@
         <v>42</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2369,12 +2399,12 @@
         <v>48</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2390,17 +2420,17 @@
         <v>2</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G29" s="5">
         <f>VLOOKUP(E29, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2633,7 +2663,7 @@
         <v>1300</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2661,7 +2691,7 @@
         <v>1300</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2689,7 +2719,7 @@
         <v>1300</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -2722,7 +2752,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B41" s="1">
         <v>2</v>
@@ -2778,7 +2808,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B43" s="1">
         <v>2</v>
@@ -2794,14 +2824,14 @@
         <v>2</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G43" s="5">
         <f>VLOOKUP(E43, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>1300</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2838,7 +2868,7 @@
         <v>42</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2875,7 +2905,7 @@
         <v>44</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -2913,7 +2943,7 @@
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -2950,7 +2980,7 @@
         <v>43</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -2987,7 +3017,7 @@
         <v>45</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -3024,7 +3054,7 @@
         <v>46</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -3052,10 +3082,10 @@
         <v>2100</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -3083,10 +3113,10 @@
         <v>2100</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -3114,10 +3144,10 @@
         <v>2100</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -3148,12 +3178,12 @@
         <v>45</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55" s="1">
         <v>2</v>
@@ -3179,7 +3209,7 @@
         <v>52</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -3210,12 +3240,12 @@
         <v>44</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B57" s="1">
         <v>2</v>
@@ -3231,17 +3261,17 @@
         <v>3</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G57" s="5">
         <f>VLOOKUP(E57, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3563,7 +3593,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B69" s="1">
         <v>3</v>
@@ -3619,7 +3649,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B71" s="1">
         <v>3</v>
@@ -3635,14 +3665,14 @@
         <v>3</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G71" s="5">
         <f>VLOOKUP(E71, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>2100</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -3679,7 +3709,7 @@
         <v>42</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -3716,7 +3746,7 @@
         <v>44</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -3754,7 +3784,7 @@
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -3791,7 +3821,7 @@
         <v>43</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -3828,7 +3858,7 @@
         <v>45</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -3865,7 +3895,7 @@
         <v>46</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -3896,7 +3926,7 @@
         <v>53</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -3927,7 +3957,7 @@
         <v>54</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -3958,7 +3988,7 @@
         <v>55</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -3989,12 +4019,12 @@
         <v>43</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B83" s="1">
         <v>3</v>
@@ -4020,7 +4050,7 @@
         <v>59</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
@@ -4051,12 +4081,12 @@
         <v>47</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B85" s="1">
         <v>3</v>
@@ -4072,17 +4102,17 @@
         <v>4</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G85" s="5">
         <f>VLOOKUP(E85, cost!$A$3:$D$15, 3, FALSE)</f>
         <v>3100</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -4093,23 +4123,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="12.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.77734375" customWidth="1"/>
+    <col min="6" max="7" width="17.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -4129,10 +4160,16 @@
         <v>60</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4150,13 +4187,19 @@
         <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -4172,16 +4215,22 @@
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A13" si="1">A3+1</f>
         <v>3</v>
@@ -4197,16 +4246,22 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4225,13 +4280,19 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>128</v>
+        <v>198</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -4250,13 +4311,19 @@
         <v>66</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>63</v>
+        <v>199</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -4275,13 +4342,19 @@
         <v>67</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>64</v>
+        <v>200</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -4300,13 +4373,19 @@
         <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>201</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -4325,13 +4404,19 @@
         <v>69</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4350,13 +4435,19 @@
         <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4375,13 +4466,19 @@
         <v>71</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -4400,13 +4497,19 @@
         <v>73</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -4422,20 +4525,26 @@
         <v>290</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>205</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" s="10"/>
     </row>
   </sheetData>
@@ -4469,16 +4578,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -4490,208 +4599,208 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3" s="19">
         <v>1</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C4" s="19">
         <v>1</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5" s="19">
         <v>3</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C7" s="19">
         <v>1</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C10" s="19">
         <v>2</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11" s="19">
         <v>2</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C13" s="19">
         <v>4</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C14" s="19">
         <v>4</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C15" s="19">
         <v>4</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C16" s="19">
         <v>4</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17" s="19">
         <v>4</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -4725,22 +4834,22 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4763,7 +4872,7 @@
         <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4784,7 +4893,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>62</v>
@@ -4859,7 +4968,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -4880,10 +4989,10 @@
         <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -4901,13 +5010,13 @@
         <v>4900</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -4925,13 +5034,13 @@
         <v>5900</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -4949,13 +5058,13 @@
         <v>7000</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4986,31 +5095,31 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="I1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -5359,7 +5468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
@@ -5381,25 +5490,25 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -5426,7 +5535,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -5482,7 +5591,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -5504,7 +5613,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -5532,13 +5641,13 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -5594,7 +5703,7 @@
         <v>3</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -5616,7 +5725,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" s="1">
         <v>3</v>
@@ -5644,13 +5753,13 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -5694,31 +5803,31 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>161</v>
-      </c>
       <c r="F1" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="J1" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -5768,7 +5877,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F3" s="14">
         <v>1</v>
@@ -5838,7 +5947,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F5" s="14">
         <v>2</v>
@@ -5881,7 +5990,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I6" s="10">
         <f xml:space="preserve"> cost!C8 - cost!C7</f>
@@ -5908,7 +6017,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F7" s="14">
         <v>2</v>
@@ -5924,7 +6033,7 @@
         <v>1300</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -5978,7 +6087,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F9" s="14">
         <v>3</v>
@@ -5987,7 +6096,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I9" s="10">
         <f xml:space="preserve"> cost!C11 - cost!C10</f>
@@ -6021,14 +6130,14 @@
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I10" s="10">
         <f xml:space="preserve"> cost!C12 - cost!C11</f>
         <v>1700</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>